<commit_message>
ajout sous menu facturation ajout facturation des mouvements
</commit_message>
<xml_diff>
--- a/facturation.xlsx
+++ b/facturation.xlsx
@@ -15,39 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>07/05/2012</t>
+    <t>01/06/2012</t>
   </si>
   <si>
-    <t>09:52:19</t>
+    <t>00:00:50</t>
   </si>
   <si>
-    <t>78opza</t>
+    <t>99aabcez</t>
   </si>
   <si>
     <t>dell300</t>
-  </si>
-  <si>
-    <t>10:15:41</t>
-  </si>
-  <si>
-    <t>dell400</t>
-  </si>
-  <si>
-    <t>08/05/2012</t>
-  </si>
-  <si>
-    <t>16:15:51</t>
-  </si>
-  <si>
-    <t>blato</t>
-  </si>
-  <si>
-    <t>cisc300</t>
   </si>
 </sst>
 </file>
@@ -387,7 +369,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
@@ -410,40 +392,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
fix generation fichier excel
</commit_message>
<xml_diff>
--- a/facturation.xlsx
+++ b/facturation.xlsx
@@ -15,57 +15,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>07/05/2012</t>
-  </si>
-  <si>
-    <t>09:52:19</t>
-  </si>
-  <si>
-    <t>78opza</t>
-  </si>
-  <si>
-    <t>dell300</t>
-  </si>
-  <si>
-    <t>10:15:41</t>
-  </si>
-  <si>
-    <t>dell400</t>
-  </si>
-  <si>
-    <t>08/05/2012</t>
-  </si>
-  <si>
-    <t>16:15:51</t>
-  </si>
-  <si>
-    <t>blato</t>
-  </si>
-  <si>
-    <t>cisc300</t>
-  </si>
-  <si>
-    <t>11/05/2012</t>
-  </si>
-  <si>
-    <t>21:11:36</t>
-  </si>
-  <si>
-    <t>cisc400</t>
-  </si>
-  <si>
-    <t>12/05/2012</t>
-  </si>
-  <si>
-    <t>09:12:34</t>
-  </si>
-  <si>
-    <t>toto</t>
+    <t>16/05/2012</t>
+  </si>
+  <si>
+    <t>12:30:08</t>
+  </si>
+  <si>
+    <t>DELL300</t>
+  </si>
+  <si>
+    <t>12:35:29</t>
+  </si>
+  <si>
+    <t>AZ123456</t>
+  </si>
+  <si>
+    <t>DELL200</t>
+  </si>
+  <si>
+    <t>13:24:02</t>
+  </si>
+  <si>
+    <t>DELL400</t>
+  </si>
+  <si>
+    <t>13:24:24</t>
+  </si>
+  <si>
+    <t>BOUY300</t>
+  </si>
+  <si>
+    <t>13:24:43</t>
+  </si>
+  <si>
+    <t>13:26:26</t>
+  </si>
+  <si>
+    <t>13:44:51</t>
+  </si>
+  <si>
+    <t>AZERTY</t>
+  </si>
+  <si>
+    <t>DELL100</t>
+  </si>
+  <si>
+    <t>16:43:40</t>
+  </si>
+  <si>
+    <t>17:19:40</t>
+  </si>
+  <si>
+    <t>DELL700</t>
+  </si>
+  <si>
+    <t>BOUY700</t>
+  </si>
+  <si>
+    <t>17:31:16</t>
+  </si>
+  <si>
+    <t>BOUY800</t>
   </si>
 </sst>
 </file>
@@ -405,7 +420,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
@@ -421,11 +436,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1">
+        <v>12345</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -436,10 +451,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -450,16 +465,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>123456</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -467,16 +482,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -484,16 +499,203 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>12345</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>12345</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
+      <c r="D8">
+        <v>12345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>12345</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>12345</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>12345</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>12345</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>